<commit_message>
move Usuarios & Contacto components to separate folders, update Contacto style
</commit_message>
<xml_diff>
--- a/src/media/EjemploContactos.xlsx
+++ b/src/media/EjemploContactos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -95,15 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">Preferido4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canal5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuenta5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preferido5</t>
   </si>
   <si>
     <t xml:space="preserve">Juan</t>
@@ -240,15 +231,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y12" activeCellId="0" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="8.36"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -324,40 +318,31 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>100</v>
@@ -369,21 +354,21 @@
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -392,9 +377,6 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>